<commit_message>
added missing DOY 206 Block 3 Bepa Data
</commit_message>
<xml_diff>
--- a/data/shoot_elongation/shoot_elongation.xlsx
+++ b/data/shoot_elongation/shoot_elongation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\my_repo_dir\fuelinex\data\shoot_elongation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1DBFD6-D1C9-4602-AE57-509486AD02A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF68E753-B7E5-40DE-A3F8-DFF4B140749D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shoot_elongation" sheetId="1" r:id="rId1"/>
@@ -3426,8 +3426,8 @@
   <dimension ref="A1:W631"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z563" sqref="Z563"/>
+      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X163" sqref="X163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -8569,6 +8569,9 @@
       <c r="U102">
         <v>7.4</v>
       </c>
+      <c r="V102">
+        <v>7.3</v>
+      </c>
       <c r="W102">
         <v>7.3</v>
       </c>
@@ -8622,6 +8625,9 @@
       <c r="U103">
         <v>12.3</v>
       </c>
+      <c r="V103">
+        <v>12.4</v>
+      </c>
       <c r="W103">
         <v>12.2</v>
       </c>
@@ -8675,6 +8681,9 @@
       <c r="U104">
         <v>8.9</v>
       </c>
+      <c r="V104">
+        <v>8.9</v>
+      </c>
       <c r="W104">
         <v>8.8000000000000007</v>
       </c>
@@ -8728,6 +8737,9 @@
       <c r="U105">
         <v>6.6</v>
       </c>
+      <c r="V105">
+        <v>6.6</v>
+      </c>
       <c r="W105">
         <v>6.5</v>
       </c>
@@ -8781,6 +8793,9 @@
       <c r="U106">
         <v>11.2</v>
       </c>
+      <c r="V106">
+        <v>11.2</v>
+      </c>
       <c r="W106">
         <v>11</v>
       </c>
@@ -9400,6 +9415,9 @@
       <c r="U117">
         <v>7.8</v>
       </c>
+      <c r="V117">
+        <v>7.8</v>
+      </c>
       <c r="W117">
         <v>7.6</v>
       </c>
@@ -9453,6 +9471,9 @@
       <c r="U118">
         <v>6.9</v>
       </c>
+      <c r="V118">
+        <v>6.7</v>
+      </c>
       <c r="W118">
         <v>6.8</v>
       </c>
@@ -9506,6 +9527,9 @@
       <c r="U119">
         <v>5.9</v>
       </c>
+      <c r="V119">
+        <v>5.9</v>
+      </c>
       <c r="W119">
         <v>6</v>
       </c>
@@ -9559,6 +9583,9 @@
       <c r="U120">
         <v>6.4</v>
       </c>
+      <c r="V120">
+        <v>6.4</v>
+      </c>
       <c r="W120">
         <v>6.4</v>
       </c>
@@ -9612,6 +9639,9 @@
       <c r="U121">
         <v>3.4</v>
       </c>
+      <c r="V121">
+        <v>3.4</v>
+      </c>
       <c r="W121">
         <v>3.4</v>
       </c>
@@ -10228,6 +10258,9 @@
       <c r="U132">
         <v>3.2</v>
       </c>
+      <c r="V132">
+        <v>3.4</v>
+      </c>
       <c r="W132">
         <v>3.5</v>
       </c>
@@ -10281,6 +10314,9 @@
       <c r="U133">
         <v>4.8</v>
       </c>
+      <c r="V133">
+        <v>4.8</v>
+      </c>
       <c r="W133">
         <v>4.7</v>
       </c>
@@ -10334,6 +10370,9 @@
       <c r="U134">
         <v>13.2</v>
       </c>
+      <c r="V134">
+        <v>13.3</v>
+      </c>
       <c r="W134">
         <v>13.3</v>
       </c>
@@ -10387,6 +10426,9 @@
       <c r="U135">
         <v>14.8</v>
       </c>
+      <c r="V135">
+        <v>14.9</v>
+      </c>
       <c r="W135">
         <v>14.8</v>
       </c>
@@ -10443,6 +10485,9 @@
       <c r="U136">
         <v>10.1</v>
       </c>
+      <c r="V136">
+        <v>10</v>
+      </c>
       <c r="W136">
         <v>10</v>
       </c>
@@ -11056,6 +11101,9 @@
       <c r="U147">
         <v>6.6</v>
       </c>
+      <c r="V147">
+        <v>6.5</v>
+      </c>
       <c r="W147">
         <v>6.4</v>
       </c>
@@ -11109,6 +11157,9 @@
       <c r="U148">
         <v>1.7</v>
       </c>
+      <c r="V148">
+        <v>1.6</v>
+      </c>
       <c r="W148">
         <v>2.1</v>
       </c>
@@ -11162,6 +11213,9 @@
       <c r="U149">
         <v>3</v>
       </c>
+      <c r="V149">
+        <v>3.1</v>
+      </c>
       <c r="W149">
         <v>3.1</v>
       </c>
@@ -11215,6 +11269,9 @@
       <c r="U150">
         <v>9.9</v>
       </c>
+      <c r="V150">
+        <v>9.9</v>
+      </c>
       <c r="W150">
         <v>9.8000000000000007</v>
       </c>
@@ -11268,6 +11325,9 @@
       <c r="U151">
         <v>11.6</v>
       </c>
+      <c r="V151">
+        <v>11.6</v>
+      </c>
       <c r="W151">
         <v>11.6</v>
       </c>
@@ -11884,6 +11944,9 @@
       <c r="U162">
         <v>5.0999999999999996</v>
       </c>
+      <c r="V162">
+        <v>5.0999999999999996</v>
+      </c>
       <c r="W162">
         <v>8.5</v>
       </c>
@@ -11937,6 +12000,9 @@
       <c r="U163">
         <v>11.3</v>
       </c>
+      <c r="V163">
+        <v>11.5</v>
+      </c>
       <c r="W163">
         <v>11.3</v>
       </c>
@@ -11993,6 +12059,9 @@
       <c r="U164">
         <v>5.4</v>
       </c>
+      <c r="V164">
+        <v>5.3</v>
+      </c>
       <c r="W164">
         <v>5.3</v>
       </c>
@@ -12046,6 +12115,9 @@
       <c r="U165">
         <v>13.4</v>
       </c>
+      <c r="V165">
+        <v>13.4</v>
+      </c>
       <c r="W165">
         <v>13.2</v>
       </c>
@@ -12099,6 +12171,9 @@
       <c r="U166">
         <v>7.1</v>
       </c>
+      <c r="V166">
+        <v>7.1</v>
+      </c>
       <c r="W166">
         <v>7.1</v>
       </c>
@@ -12712,6 +12787,9 @@
       <c r="U177">
         <v>4.2</v>
       </c>
+      <c r="V177">
+        <v>4.4000000000000004</v>
+      </c>
       <c r="W177">
         <v>4.2</v>
       </c>
@@ -12765,6 +12843,9 @@
       <c r="U178">
         <v>9.6999999999999993</v>
       </c>
+      <c r="V178">
+        <v>9.6999999999999993</v>
+      </c>
       <c r="W178">
         <v>9.6</v>
       </c>
@@ -12818,6 +12899,9 @@
       <c r="U179">
         <v>8.9</v>
       </c>
+      <c r="V179">
+        <v>9.1</v>
+      </c>
       <c r="W179">
         <v>8.9</v>
       </c>
@@ -12871,6 +12955,9 @@
       <c r="U180">
         <v>14.8</v>
       </c>
+      <c r="V180">
+        <v>14.2</v>
+      </c>
       <c r="W180">
         <v>14.8</v>
       </c>
@@ -12922,6 +13009,9 @@
         <v>6.1</v>
       </c>
       <c r="U181">
+        <v>6.1</v>
+      </c>
+      <c r="V181">
         <v>6.1</v>
       </c>
       <c r="W181">

</xml_diff>